<commit_message>
Auto-committed on 2023/02/21 週二 11:59:01.76
</commit_message>
<xml_diff>
--- a/Program/Other/LM001_底稿_公會報送無自用住宅統計.xlsx
+++ b/Program/Other/LM001_底稿_公會報送無自用住宅統計.xlsx
@@ -5,10 +5,10 @@
   <workbookPr checkCompatibility="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\st1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B56413-41E0-4FE5-A5AB-4B80C78A066F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25A7683-282A-4F23-847E-78A3FD5AF95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,7 +756,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -853,6 +852,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1195,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
@@ -1209,54 +1211,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" ht="17.5" thickBot="1">
-      <c r="A3" s="25"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:8" ht="17.5" thickTop="1">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="32"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
@@ -1283,10 +1285,10 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
@@ -1295,10 +1297,10 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" ht="17.5" thickBot="1">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="15"/>
@@ -1307,22 +1309,22 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" ht="17.5" thickTop="1">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
       <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -1331,10 +1333,10 @@
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -1343,10 +1345,10 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="28"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -1355,10 +1357,10 @@
       <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="34"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -1367,10 +1369,10 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -1379,10 +1381,10 @@
       <c r="H13" s="17"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="34"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -1391,10 +1393,10 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:8" ht="17.5" thickBot="1">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="36"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="20"/>
@@ -1408,80 +1410,80 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8" ht="17.5" thickBot="1">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
     </row>
     <row r="19" spans="1:8" ht="17.5" thickTop="1">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="42"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="41"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="44"/>
-      <c r="E20" s="46" t="s">
+      <c r="D20" s="43"/>
+      <c r="E20" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="44"/>
-      <c r="G20" s="45" t="s">
+      <c r="F20" s="43"/>
+      <c r="G20" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="47"/>
+      <c r="H20" s="46"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="48"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="56"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="55"/>
     </row>
     <row r="22" spans="1:8" ht="17.5" thickBot="1">
-      <c r="A22" s="35"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="58"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="57"/>
     </row>
     <row r="23" spans="1:8" s="23" customFormat="1" ht="17.5" thickTop="1">
       <c r="C23" s="23" t="s">
@@ -1526,7 +1528,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="27">
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="E20:F20"/>
@@ -1553,6 +1555,7 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -1566,6 +1569,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x0101002F834950E6E8EC4987003F88DFC9B5CE" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="f8649297cceefdfdcd508960509e4249">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="684b3c36135c6fbac31a56fab451a81a">
     <xsd:element name="properties">
@@ -1679,22 +1697,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE61CA3A-D0AF-4EBD-9CD1-5CE8BB8E6662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F52CE6E3-4712-449A-9578-42DFEA61DDE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{133E6AC9-7FB7-4D4C-A75A-5AB39B147B6A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1708,21 +1728,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE61CA3A-D0AF-4EBD-9CD1-5CE8BB8E6662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F52CE6E3-4712-449A-9578-42DFEA61DDE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>